<commit_message>
fixed unit tests errors
</commit_message>
<xml_diff>
--- a/ExampleCase.xlsx
+++ b/ExampleCase.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="227">
   <si>
     <t>uuid</t>
   </si>
@@ -411,9 +411,6 @@
   </si>
   <si>
     <t>2021-02-04 12:00:00</t>
-  </si>
-  <si>
-    <t>-20.28</t>
   </si>
   <si>
     <t>0.86</t>
@@ -1824,777 +1821,777 @@
         <v>96</v>
       </c>
       <c r="D8" t="s" s="1">
-        <v>133</v>
+        <v>91</v>
       </c>
       <c r="E8" t="s" s="1">
         <v>101</v>
       </c>
       <c r="F8" t="s" s="1">
+        <v>133</v>
+      </c>
+      <c r="G8" t="s" s="1">
         <v>134</v>
-      </c>
-      <c r="G8" t="s" s="1">
-        <v>135</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="4">
+        <v>135</v>
+      </c>
+      <c r="B10" t="s" s="4">
         <v>136</v>
       </c>
-      <c r="B10" t="s" s="4">
+      <c r="C10" t="s" s="4">
         <v>137</v>
       </c>
-      <c r="C10" t="s" s="4">
+      <c r="D10" t="s" s="4">
         <v>138</v>
-      </c>
-      <c r="D10" t="s" s="4">
-        <v>139</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B11" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C11" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D11" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D12" t="s" s="1">
         <v>142</v>
-      </c>
-      <c r="B12" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C12" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D12" t="s" s="1">
-        <v>143</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="1">
+        <v>143</v>
+      </c>
+      <c r="B13" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D13" t="s" s="1">
         <v>144</v>
-      </c>
-      <c r="B13" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C13" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D13" t="s" s="1">
-        <v>145</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="1">
+        <v>145</v>
+      </c>
+      <c r="B14" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C14" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D14" t="s" s="1">
         <v>146</v>
-      </c>
-      <c r="B14" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C14" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D14" t="s" s="1">
-        <v>147</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="1">
+        <v>147</v>
+      </c>
+      <c r="B15" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C15" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D15" t="s" s="1">
         <v>148</v>
-      </c>
-      <c r="B15" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C15" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D15" t="s" s="1">
-        <v>149</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="1">
+        <v>149</v>
+      </c>
+      <c r="B16" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D16" t="s" s="1">
         <v>150</v>
-      </c>
-      <c r="B16" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C16" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D16" t="s" s="1">
-        <v>151</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
+        <v>151</v>
+      </c>
+      <c r="B17" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D17" t="s" s="1">
         <v>152</v>
-      </c>
-      <c r="B17" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C17" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D17" t="s" s="1">
-        <v>153</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
+        <v>153</v>
+      </c>
+      <c r="B18" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C18" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D18" t="s" s="1">
         <v>154</v>
-      </c>
-      <c r="B18" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C18" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D18" t="s" s="1">
-        <v>155</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
+        <v>155</v>
+      </c>
+      <c r="B19" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D19" t="s" s="1">
         <v>156</v>
-      </c>
-      <c r="B19" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C19" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D19" t="s" s="1">
-        <v>157</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
+        <v>157</v>
+      </c>
+      <c r="B20" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D20" t="s" s="1">
         <v>158</v>
-      </c>
-      <c r="B20" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C20" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D20" t="s" s="1">
-        <v>159</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
+        <v>159</v>
+      </c>
+      <c r="B21" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C21" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D21" t="s" s="1">
         <v>160</v>
-      </c>
-      <c r="B21" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C21" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D21" t="s" s="1">
-        <v>161</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
+        <v>161</v>
+      </c>
+      <c r="B22" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D22" t="s" s="1">
         <v>162</v>
-      </c>
-      <c r="B22" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C22" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D22" t="s" s="1">
-        <v>163</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
+        <v>163</v>
+      </c>
+      <c r="B23" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D23" t="s" s="1">
         <v>164</v>
-      </c>
-      <c r="B23" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C23" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D23" t="s" s="1">
-        <v>165</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
+        <v>165</v>
+      </c>
+      <c r="B24" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C24" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D24" t="s" s="1">
         <v>166</v>
-      </c>
-      <c r="B24" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C24" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D24" t="s" s="1">
-        <v>167</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
+        <v>167</v>
+      </c>
+      <c r="B25" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D25" t="s" s="1">
         <v>168</v>
-      </c>
-      <c r="B25" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C25" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D25" t="s" s="1">
-        <v>169</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
+        <v>169</v>
+      </c>
+      <c r="B26" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D26" t="s" s="1">
         <v>170</v>
-      </c>
-      <c r="B26" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C26" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D26" t="s" s="1">
-        <v>171</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="1">
+        <v>171</v>
+      </c>
+      <c r="B27" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D27" t="s" s="1">
         <v>172</v>
-      </c>
-      <c r="B27" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C27" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D27" t="s" s="1">
-        <v>173</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="1">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B28" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C28" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D28" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="1">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B29" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C29" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D29" t="s" s="1">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B30" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C30" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D30" t="s" s="1">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="1">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B31" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C31" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D31" t="s" s="1">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="1">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B32" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C32" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D32" t="s" s="1">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="1">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B33" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C33" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D33" t="s" s="1">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="1">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B34" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C34" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D34" t="s" s="1">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="1">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B35" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C35" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D35" t="s" s="1">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="1">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B36" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C36" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D36" t="s" s="1">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="1">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B37" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C37" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D37" t="s" s="1">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="1">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B38" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C38" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D38" t="s" s="1">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="1">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B39" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C39" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D39" t="s" s="1">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="1">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B40" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C40" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D40" t="s" s="1">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="1">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B41" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C41" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D41" t="s" s="1">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="1">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B42" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C42" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D42" t="s" s="1">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="1">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B43" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C43" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D43" t="s" s="1">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="1">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B44" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C44" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D44" t="s" s="1">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B45" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C45" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D45" t="s" s="1">
         <v>191</v>
-      </c>
-      <c r="B45" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C45" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D45" t="s" s="1">
-        <v>192</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="1">
+        <v>192</v>
+      </c>
+      <c r="B46" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C46" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D46" t="s" s="1">
         <v>193</v>
-      </c>
-      <c r="B46" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C46" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D46" t="s" s="1">
-        <v>194</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="1">
+        <v>194</v>
+      </c>
+      <c r="B47" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C47" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D47" t="s" s="1">
         <v>195</v>
-      </c>
-      <c r="B47" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C47" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D47" t="s" s="1">
-        <v>196</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="1">
+        <v>196</v>
+      </c>
+      <c r="B48" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C48" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D48" t="s" s="1">
         <v>197</v>
-      </c>
-      <c r="B48" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C48" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D48" t="s" s="1">
-        <v>198</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="1">
+        <v>198</v>
+      </c>
+      <c r="B49" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C49" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D49" t="s" s="1">
         <v>199</v>
-      </c>
-      <c r="B49" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C49" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D49" t="s" s="1">
-        <v>200</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="1">
+        <v>200</v>
+      </c>
+      <c r="B50" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C50" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D50" t="s" s="1">
         <v>201</v>
-      </c>
-      <c r="B50" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C50" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D50" t="s" s="1">
-        <v>202</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="1">
+        <v>202</v>
+      </c>
+      <c r="B51" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C51" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D51" t="s" s="1">
         <v>203</v>
-      </c>
-      <c r="B51" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C51" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D51" t="s" s="1">
-        <v>204</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="1">
+        <v>204</v>
+      </c>
+      <c r="B52" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C52" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D52" t="s" s="1">
         <v>205</v>
-      </c>
-      <c r="B52" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C52" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D52" t="s" s="1">
-        <v>206</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="1">
+        <v>206</v>
+      </c>
+      <c r="B53" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C53" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D53" t="s" s="1">
         <v>207</v>
-      </c>
-      <c r="B53" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C53" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D53" t="s" s="1">
-        <v>208</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="1">
+        <v>208</v>
+      </c>
+      <c r="B54" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C54" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D54" t="s" s="1">
         <v>209</v>
-      </c>
-      <c r="B54" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C54" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D54" t="s" s="1">
-        <v>210</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="1">
+        <v>210</v>
+      </c>
+      <c r="B55" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C55" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D55" t="s" s="1">
         <v>211</v>
-      </c>
-      <c r="B55" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C55" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D55" t="s" s="1">
-        <v>212</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="1">
+        <v>212</v>
+      </c>
+      <c r="B56" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C56" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D56" t="s" s="1">
         <v>213</v>
-      </c>
-      <c r="B56" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C56" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D56" t="s" s="1">
-        <v>214</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="1">
+        <v>214</v>
+      </c>
+      <c r="B57" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C57" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D57" t="s" s="1">
         <v>215</v>
-      </c>
-      <c r="B57" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C57" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D57" t="s" s="1">
-        <v>216</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="1">
+        <v>216</v>
+      </c>
+      <c r="B58" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C58" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="D58" t="s" s="1">
         <v>217</v>
-      </c>
-      <c r="B58" t="s" s="1">
-        <v>96</v>
-      </c>
-      <c r="C58" t="s" s="1">
-        <v>141</v>
-      </c>
-      <c r="D58" t="s" s="1">
-        <v>218</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="1">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B59" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C59" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D59" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="1">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B60" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C60" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D60" t="s" s="1">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="1">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B61" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C61" t="s" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D61" t="s" s="1">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="5">
+        <v>221</v>
+      </c>
+      <c r="B63" t="s" s="5">
         <v>222</v>
       </c>
-      <c r="B63" t="s" s="5">
+      <c r="C63" t="s" s="5">
         <v>223</v>
-      </c>
-      <c r="C63" t="s" s="5">
-        <v>224</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="1">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B64" t="s" s="1">
+        <v>224</v>
+      </c>
+      <c r="C64" t="s" s="1">
         <v>225</v>
-      </c>
-      <c r="C64" t="s" s="1">
-        <v>226</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="1">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B65" t="s" s="1">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C65" t="s" s="1">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes for monitoring and payment
</commit_message>
<xml_diff>
--- a/ExampleCase.xlsx
+++ b/ExampleCase.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="231">
   <si>
     <t>uuid</t>
   </si>
@@ -404,6 +404,9 @@
     <t>Rejection Date</t>
   </si>
   <si>
+    <t>Rejection Code</t>
+  </si>
+  <si>
     <t>Daily Benefit</t>
   </si>
   <si>
@@ -413,6 +416,9 @@
     <t>2021-02-04 12:00:00</t>
   </si>
   <si>
+    <t>REJECTION0</t>
+  </si>
+  <si>
     <t>0.86</t>
   </si>
   <si>
@@ -683,10 +689,16 @@
     <t>Payment State</t>
   </si>
   <si>
-    <t>Payment Value</t>
+    <t>Calculated Payment</t>
+  </si>
+  <si>
+    <t>Actual Payment Value</t>
   </si>
   <si>
     <t>PAID</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
   <si>
     <t>0.51</t>
@@ -772,92 +784,92 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="26.11328125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="26.11328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="85.20703125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="85.20703125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="29.1484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="30.01171875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="35.1953125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="32.140625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="36.734375" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="37.59765625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="17.44140625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="26.984375" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="19.953125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="17.98828125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="22.28125" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="20.04296875" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="31.828125" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="10.01171875" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="11.21484375" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="10.796875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="22.73828125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="5.46875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.609375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="17.35546875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="18.9609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="22.65625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="25.56640625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="23.48828125" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="12.37890625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="25.359375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="27.26953125" customWidth="true" bestFit="true"/>
-    <col min="32" max="32" width="30.2265625" customWidth="true" bestFit="true"/>
-    <col min="33" max="33" width="20.22265625" customWidth="true" bestFit="true"/>
-    <col min="34" max="34" width="16.42578125" customWidth="true" bestFit="true"/>
-    <col min="35" max="35" width="11.98046875" customWidth="true" bestFit="true"/>
-    <col min="36" max="36" width="16.17578125" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="9.9453125" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="21.27734375" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="13.78515625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="15.27734375" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="25.9296875" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="20.796875" customWidth="true" bestFit="true"/>
-    <col min="43" max="43" width="20.26171875" customWidth="true" bestFit="true"/>
-    <col min="44" max="44" width="19.20703125" customWidth="true" bestFit="true"/>
-    <col min="45" max="45" width="13.55078125" customWidth="true" bestFit="true"/>
-    <col min="46" max="46" width="26.5390625" customWidth="true" bestFit="true"/>
-    <col min="47" max="47" width="15.5078125" customWidth="true" bestFit="true"/>
-    <col min="48" max="48" width="17.21875" customWidth="true" bestFit="true"/>
-    <col min="49" max="49" width="15.55859375" customWidth="true" bestFit="true"/>
-    <col min="50" max="50" width="17.875" customWidth="true" bestFit="true"/>
-    <col min="51" max="51" width="20.96875" customWidth="true" bestFit="true"/>
-    <col min="52" max="52" width="37.21875" customWidth="true" bestFit="true"/>
-    <col min="53" max="53" width="24.39453125" customWidth="true" bestFit="true"/>
-    <col min="54" max="54" width="10.75" customWidth="true" bestFit="true"/>
-    <col min="55" max="55" width="22.80078125" customWidth="true" bestFit="true"/>
-    <col min="56" max="56" width="15.234375" customWidth="true" bestFit="true"/>
-    <col min="57" max="57" width="26.98828125" customWidth="true" bestFit="true"/>
-    <col min="58" max="58" width="16.61328125" customWidth="true" bestFit="true"/>
-    <col min="59" max="59" width="33.62109375" customWidth="true" bestFit="true"/>
-    <col min="60" max="60" width="30.7734375" customWidth="true" bestFit="true"/>
-    <col min="61" max="61" width="22.94140625" customWidth="true" bestFit="true"/>
-    <col min="62" max="62" width="22.36328125" customWidth="true" bestFit="true"/>
-    <col min="63" max="63" width="19.71484375" customWidth="true" bestFit="true"/>
-    <col min="64" max="64" width="17.5859375" customWidth="true" bestFit="true"/>
-    <col min="65" max="65" width="13.76171875" customWidth="true" bestFit="true"/>
-    <col min="66" max="66" width="35.4921875" customWidth="true" bestFit="true"/>
-    <col min="67" max="67" width="14.890625" customWidth="true" bestFit="true"/>
-    <col min="68" max="68" width="54.09765625" customWidth="true" bestFit="true"/>
-    <col min="69" max="69" width="213.13671875" customWidth="true" bestFit="true"/>
-    <col min="70" max="70" width="213.13671875" customWidth="true" bestFit="true"/>
-    <col min="71" max="71" width="36.74609375" customWidth="true" bestFit="true"/>
-    <col min="72" max="72" width="28.109375" customWidth="true" bestFit="true"/>
-    <col min="73" max="73" width="26.44921875" customWidth="true" bestFit="true"/>
-    <col min="74" max="74" width="69.1953125" customWidth="true" bestFit="true"/>
-    <col min="75" max="75" width="66.22265625" customWidth="true" bestFit="true"/>
-    <col min="76" max="76" width="33.77734375" customWidth="true" bestFit="true"/>
-    <col min="77" max="77" width="44.51171875" customWidth="true" bestFit="true"/>
-    <col min="78" max="78" width="41.6640625" customWidth="true" bestFit="true"/>
-    <col min="79" max="79" width="48.109375" customWidth="true" bestFit="true"/>
-    <col min="80" max="80" width="29.85546875" customWidth="true" bestFit="true"/>
-    <col min="81" max="81" width="22.90234375" customWidth="true" bestFit="true"/>
-    <col min="82" max="82" width="24.953125" customWidth="true" bestFit="true"/>
-    <col min="83" max="83" width="18.94921875" customWidth="true" bestFit="true"/>
-    <col min="84" max="84" width="20.7734375" customWidth="true" bestFit="true"/>
-    <col min="85" max="85" width="14.33984375" customWidth="true" bestFit="true"/>
-    <col min="86" max="86" width="2.07421875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="25.03515625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="25.03515625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="81.5" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="81.5" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="25.55859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="27.02734375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="30.94140625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="27.98046875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="32.1015625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="33.5703125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="15.4140625" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="23.79296875" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="17.58984375" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="15.94140625" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="19.421875" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="17.61328125" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="27.71484375" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" width="9.109375" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="9.390625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="20.28125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="4.97265625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="15.5390625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="15.6015625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="16.69140625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="20.5" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="22.3828125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.59375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="10.84375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="21.8984375" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="24.265625" customWidth="true" bestFit="true"/>
+    <col min="32" max="32" width="26.83203125" customWidth="true" bestFit="true"/>
+    <col min="33" max="33" width="18.25" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="14.81640625" customWidth="true" bestFit="true"/>
+    <col min="35" max="35" width="10.734375" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="14.48046875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="8.8984375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="19.2265625" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="12.234375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="14.76171875" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="23.5" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="18.75390625" customWidth="true" bestFit="true"/>
+    <col min="43" max="43" width="17.9765625" customWidth="true" bestFit="true"/>
+    <col min="44" max="44" width="17.28125" customWidth="true" bestFit="true"/>
+    <col min="45" max="45" width="11.9296875" customWidth="true" bestFit="true"/>
+    <col min="46" max="46" width="23.578125" customWidth="true" bestFit="true"/>
+    <col min="47" max="47" width="13.3671875" customWidth="true" bestFit="true"/>
+    <col min="48" max="48" width="15.15625" customWidth="true" bestFit="true"/>
+    <col min="49" max="49" width="13.6875" customWidth="true" bestFit="true"/>
+    <col min="50" max="50" width="15.7421875" customWidth="true" bestFit="true"/>
+    <col min="51" max="51" width="18.75390625" customWidth="true" bestFit="true"/>
+    <col min="52" max="52" width="33.40625" customWidth="true" bestFit="true"/>
+    <col min="53" max="53" width="21.546875" customWidth="true" bestFit="true"/>
+    <col min="54" max="54" width="9.33984375" customWidth="true" bestFit="true"/>
+    <col min="55" max="55" width="20.4765625" customWidth="true" bestFit="true"/>
+    <col min="56" max="56" width="13.53515625" customWidth="true" bestFit="true"/>
+    <col min="57" max="57" width="23.8359375" customWidth="true" bestFit="true"/>
+    <col min="58" max="58" width="14.6875" customWidth="true" bestFit="true"/>
+    <col min="59" max="59" width="29.66015625" customWidth="true" bestFit="true"/>
+    <col min="60" max="60" width="27.0" customWidth="true" bestFit="true"/>
+    <col min="61" max="61" width="20.421875" customWidth="true" bestFit="true"/>
+    <col min="62" max="62" width="19.8046875" customWidth="true" bestFit="true"/>
+    <col min="63" max="63" width="17.68359375" customWidth="true" bestFit="true"/>
+    <col min="64" max="64" width="15.5390625" customWidth="true" bestFit="true"/>
+    <col min="65" max="65" width="13.1953125" customWidth="true" bestFit="true"/>
+    <col min="66" max="66" width="31.81640625" customWidth="true" bestFit="true"/>
+    <col min="67" max="67" width="14.390625" customWidth="true" bestFit="true"/>
+    <col min="68" max="68" width="52.95703125" customWidth="true" bestFit="true"/>
+    <col min="69" max="69" width="210.8828125" customWidth="true" bestFit="true"/>
+    <col min="70" max="70" width="210.8828125" customWidth="true" bestFit="true"/>
+    <col min="71" max="71" width="34.7890625" customWidth="true" bestFit="true"/>
+    <col min="72" max="72" width="24.72265625" customWidth="true" bestFit="true"/>
+    <col min="73" max="73" width="23.25390625" customWidth="true" bestFit="true"/>
+    <col min="74" max="74" width="65.421875" customWidth="true" bestFit="true"/>
+    <col min="75" max="75" width="62.58203125" customWidth="true" bestFit="true"/>
+    <col min="76" max="76" width="31.953125" customWidth="true" bestFit="true"/>
+    <col min="77" max="77" width="39.2265625" customWidth="true" bestFit="true"/>
+    <col min="78" max="78" width="36.5625" customWidth="true" bestFit="true"/>
+    <col min="79" max="79" width="42.96875" customWidth="true" bestFit="true"/>
+    <col min="80" max="80" width="26.8046875" customWidth="true" bestFit="true"/>
+    <col min="81" max="81" width="20.8984375" customWidth="true" bestFit="true"/>
+    <col min="82" max="82" width="22.546875" customWidth="true" bestFit="true"/>
+    <col min="83" max="83" width="17.14453125" customWidth="true" bestFit="true"/>
+    <col min="84" max="84" width="18.75390625" customWidth="true" bestFit="true"/>
+    <col min="85" max="85" width="12.8203125" customWidth="true" bestFit="true"/>
+    <col min="86" max="86" width="1.953125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1809,13 +1821,16 @@
       <c r="G7" t="s" s="3">
         <v>131</v>
       </c>
+      <c r="H7" t="s" s="3">
+        <v>132</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
         <v>85</v>
       </c>
       <c r="B8" t="s" s="1">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s" s="1">
         <v>96</v>
@@ -1827,771 +1842,783 @@
         <v>101</v>
       </c>
       <c r="F8" t="s" s="1">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G8" t="s" s="1">
-        <v>134</v>
+        <v>135</v>
+      </c>
+      <c r="H8" t="s" s="1">
+        <v>136</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="4">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C11" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D11" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C12" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D12" t="s" s="1">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="1">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B13" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C13" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D13" t="s" s="1">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="1">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B14" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C14" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D14" t="s" s="1">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="1">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B15" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C15" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D15" t="s" s="1">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="1">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C16" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D16" t="s" s="1">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B17" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C17" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D17" t="s" s="1">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B18" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C18" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D18" t="s" s="1">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B19" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C19" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D19" t="s" s="1">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B20" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C20" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D20" t="s" s="1">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B21" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C21" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D21" t="s" s="1">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B22" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C22" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D22" t="s" s="1">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B23" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C23" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D23" t="s" s="1">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B24" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C24" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D24" t="s" s="1">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B25" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C25" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D25" t="s" s="1">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B26" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C26" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D26" t="s" s="1">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="1">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B27" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C27" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D27" t="s" s="1">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="1">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B28" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C28" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D28" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="1">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B29" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C29" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D29" t="s" s="1">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B30" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C30" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D30" t="s" s="1">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="1">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B31" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C31" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D31" t="s" s="1">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="1">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B32" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C32" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D32" t="s" s="1">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="1">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B33" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C33" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D33" t="s" s="1">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="1">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B34" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C34" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D34" t="s" s="1">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="1">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B35" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C35" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D35" t="s" s="1">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="1">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C36" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D36" t="s" s="1">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="1">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C37" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D37" t="s" s="1">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="1">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B38" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C38" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D38" t="s" s="1">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="1">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B39" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C39" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D39" t="s" s="1">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="1">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B40" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C40" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D40" t="s" s="1">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="1">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B41" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C41" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D41" t="s" s="1">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="1">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B42" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C42" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D42" t="s" s="1">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="1">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B43" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C43" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D43" t="s" s="1">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="1">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B44" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C44" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D44" t="s" s="1">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="1">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B45" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C45" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D45" t="s" s="1">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="1">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B46" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C46" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D46" t="s" s="1">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="1">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B47" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C47" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D47" t="s" s="1">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="1">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B48" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C48" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D48" t="s" s="1">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="1">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B49" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C49" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D49" t="s" s="1">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="1">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B50" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C50" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D50" t="s" s="1">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="1">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B51" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C51" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D51" t="s" s="1">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="1">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B52" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C52" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D52" t="s" s="1">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="1">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B53" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C53" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D53" t="s" s="1">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="1">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B54" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C54" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D54" t="s" s="1">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="1">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B55" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C55" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D55" t="s" s="1">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="1">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B56" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C56" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D56" t="s" s="1">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="1">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B57" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C57" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D57" t="s" s="1">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="1">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B58" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C58" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D58" t="s" s="1">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="1">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B59" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C59" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D59" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="1">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B60" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C60" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D60" t="s" s="1">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="1">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B61" t="s" s="1">
         <v>96</v>
       </c>
       <c r="C61" t="s" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D61" t="s" s="1">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="5">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B63" t="s" s="5">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C63" t="s" s="5">
-        <v>223</v>
+        <v>225</v>
+      </c>
+      <c r="D63" t="s" s="5">
+        <v>226</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="1">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B64" t="s" s="1">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C64" t="s" s="1">
-        <v>225</v>
+        <v>228</v>
+      </c>
+      <c r="D64" t="s" s="1">
+        <v>229</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="1">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B65" t="s" s="1">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C65" t="s" s="1">
-        <v>226</v>
+        <v>228</v>
+      </c>
+      <c r="D65" t="s" s="1">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generate and upload interfaces
</commit_message>
<xml_diff>
--- a/ExampleCase.xlsx
+++ b/ExampleCase.xlsx
@@ -784,92 +784,92 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="25.03515625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="25.03515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="81.5" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="81.5" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="25.55859375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="27.02734375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="30.94140625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="27.98046875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="32.1015625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="33.5703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="15.4140625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="23.79296875" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="17.58984375" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="15.94140625" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="19.421875" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="17.61328125" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="27.71484375" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="9.109375" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="9.87890625" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.390625" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="20.28125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="4.97265625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="15.5390625" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="15.6015625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="16.69140625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="20.5" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="22.3828125" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="20.59375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="10.84375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="21.8984375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="24.265625" customWidth="true" bestFit="true"/>
-    <col min="32" max="32" width="26.83203125" customWidth="true" bestFit="true"/>
-    <col min="33" max="33" width="18.25" customWidth="true" bestFit="true"/>
-    <col min="34" max="34" width="14.81640625" customWidth="true" bestFit="true"/>
-    <col min="35" max="35" width="10.734375" customWidth="true" bestFit="true"/>
-    <col min="36" max="36" width="14.48046875" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="8.8984375" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="19.2265625" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="12.234375" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="14.76171875" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="23.5" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="18.75390625" customWidth="true" bestFit="true"/>
-    <col min="43" max="43" width="17.9765625" customWidth="true" bestFit="true"/>
-    <col min="44" max="44" width="17.28125" customWidth="true" bestFit="true"/>
-    <col min="45" max="45" width="11.9296875" customWidth="true" bestFit="true"/>
-    <col min="46" max="46" width="23.578125" customWidth="true" bestFit="true"/>
-    <col min="47" max="47" width="13.3671875" customWidth="true" bestFit="true"/>
-    <col min="48" max="48" width="15.15625" customWidth="true" bestFit="true"/>
-    <col min="49" max="49" width="13.6875" customWidth="true" bestFit="true"/>
-    <col min="50" max="50" width="15.7421875" customWidth="true" bestFit="true"/>
-    <col min="51" max="51" width="18.75390625" customWidth="true" bestFit="true"/>
-    <col min="52" max="52" width="33.40625" customWidth="true" bestFit="true"/>
-    <col min="53" max="53" width="21.546875" customWidth="true" bestFit="true"/>
-    <col min="54" max="54" width="9.33984375" customWidth="true" bestFit="true"/>
-    <col min="55" max="55" width="20.4765625" customWidth="true" bestFit="true"/>
-    <col min="56" max="56" width="13.53515625" customWidth="true" bestFit="true"/>
-    <col min="57" max="57" width="23.8359375" customWidth="true" bestFit="true"/>
-    <col min="58" max="58" width="14.6875" customWidth="true" bestFit="true"/>
-    <col min="59" max="59" width="29.66015625" customWidth="true" bestFit="true"/>
-    <col min="60" max="60" width="27.0" customWidth="true" bestFit="true"/>
-    <col min="61" max="61" width="20.421875" customWidth="true" bestFit="true"/>
-    <col min="62" max="62" width="19.8046875" customWidth="true" bestFit="true"/>
-    <col min="63" max="63" width="17.68359375" customWidth="true" bestFit="true"/>
-    <col min="64" max="64" width="15.5390625" customWidth="true" bestFit="true"/>
-    <col min="65" max="65" width="13.1953125" customWidth="true" bestFit="true"/>
-    <col min="66" max="66" width="31.81640625" customWidth="true" bestFit="true"/>
-    <col min="67" max="67" width="14.390625" customWidth="true" bestFit="true"/>
-    <col min="68" max="68" width="52.95703125" customWidth="true" bestFit="true"/>
-    <col min="69" max="69" width="210.8828125" customWidth="true" bestFit="true"/>
-    <col min="70" max="70" width="210.8828125" customWidth="true" bestFit="true"/>
-    <col min="71" max="71" width="34.7890625" customWidth="true" bestFit="true"/>
-    <col min="72" max="72" width="24.72265625" customWidth="true" bestFit="true"/>
-    <col min="73" max="73" width="23.25390625" customWidth="true" bestFit="true"/>
-    <col min="74" max="74" width="65.421875" customWidth="true" bestFit="true"/>
-    <col min="75" max="75" width="62.58203125" customWidth="true" bestFit="true"/>
-    <col min="76" max="76" width="31.953125" customWidth="true" bestFit="true"/>
-    <col min="77" max="77" width="39.2265625" customWidth="true" bestFit="true"/>
-    <col min="78" max="78" width="36.5625" customWidth="true" bestFit="true"/>
-    <col min="79" max="79" width="42.96875" customWidth="true" bestFit="true"/>
-    <col min="80" max="80" width="26.8046875" customWidth="true" bestFit="true"/>
-    <col min="81" max="81" width="20.8984375" customWidth="true" bestFit="true"/>
-    <col min="82" max="82" width="22.546875" customWidth="true" bestFit="true"/>
-    <col min="83" max="83" width="17.14453125" customWidth="true" bestFit="true"/>
-    <col min="84" max="84" width="18.75390625" customWidth="true" bestFit="true"/>
-    <col min="85" max="85" width="12.8203125" customWidth="true" bestFit="true"/>
-    <col min="86" max="86" width="1.953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="26.11328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="26.11328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="85.20703125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="85.20703125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="29.1484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="30.01171875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="35.1953125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="32.140625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="36.734375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="37.59765625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="17.44140625" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="26.984375" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="19.953125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="17.98828125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="22.28125" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="20.04296875" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="31.828125" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" width="10.01171875" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="11.21484375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="10.796875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="22.73828125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="5.46875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.609375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="17.35546875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="18.9609375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="22.65625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="25.56640625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="23.48828125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="12.37890625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="25.359375" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="27.26953125" customWidth="true" bestFit="true"/>
+    <col min="32" max="32" width="30.2265625" customWidth="true" bestFit="true"/>
+    <col min="33" max="33" width="20.22265625" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="16.42578125" customWidth="true" bestFit="true"/>
+    <col min="35" max="35" width="11.98046875" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="16.17578125" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="9.9453125" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="21.27734375" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="13.78515625" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="15.27734375" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="25.9296875" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="20.796875" customWidth="true" bestFit="true"/>
+    <col min="43" max="43" width="20.26171875" customWidth="true" bestFit="true"/>
+    <col min="44" max="44" width="19.20703125" customWidth="true" bestFit="true"/>
+    <col min="45" max="45" width="13.55078125" customWidth="true" bestFit="true"/>
+    <col min="46" max="46" width="26.5390625" customWidth="true" bestFit="true"/>
+    <col min="47" max="47" width="15.5078125" customWidth="true" bestFit="true"/>
+    <col min="48" max="48" width="17.21875" customWidth="true" bestFit="true"/>
+    <col min="49" max="49" width="15.55859375" customWidth="true" bestFit="true"/>
+    <col min="50" max="50" width="17.875" customWidth="true" bestFit="true"/>
+    <col min="51" max="51" width="20.96875" customWidth="true" bestFit="true"/>
+    <col min="52" max="52" width="37.21875" customWidth="true" bestFit="true"/>
+    <col min="53" max="53" width="24.39453125" customWidth="true" bestFit="true"/>
+    <col min="54" max="54" width="10.75" customWidth="true" bestFit="true"/>
+    <col min="55" max="55" width="22.80078125" customWidth="true" bestFit="true"/>
+    <col min="56" max="56" width="15.234375" customWidth="true" bestFit="true"/>
+    <col min="57" max="57" width="26.98828125" customWidth="true" bestFit="true"/>
+    <col min="58" max="58" width="16.61328125" customWidth="true" bestFit="true"/>
+    <col min="59" max="59" width="33.62109375" customWidth="true" bestFit="true"/>
+    <col min="60" max="60" width="30.7734375" customWidth="true" bestFit="true"/>
+    <col min="61" max="61" width="22.94140625" customWidth="true" bestFit="true"/>
+    <col min="62" max="62" width="22.36328125" customWidth="true" bestFit="true"/>
+    <col min="63" max="63" width="19.71484375" customWidth="true" bestFit="true"/>
+    <col min="64" max="64" width="17.5859375" customWidth="true" bestFit="true"/>
+    <col min="65" max="65" width="13.76171875" customWidth="true" bestFit="true"/>
+    <col min="66" max="66" width="35.4921875" customWidth="true" bestFit="true"/>
+    <col min="67" max="67" width="14.890625" customWidth="true" bestFit="true"/>
+    <col min="68" max="68" width="54.09765625" customWidth="true" bestFit="true"/>
+    <col min="69" max="69" width="213.13671875" customWidth="true" bestFit="true"/>
+    <col min="70" max="70" width="213.13671875" customWidth="true" bestFit="true"/>
+    <col min="71" max="71" width="36.74609375" customWidth="true" bestFit="true"/>
+    <col min="72" max="72" width="28.109375" customWidth="true" bestFit="true"/>
+    <col min="73" max="73" width="26.44921875" customWidth="true" bestFit="true"/>
+    <col min="74" max="74" width="69.1953125" customWidth="true" bestFit="true"/>
+    <col min="75" max="75" width="66.22265625" customWidth="true" bestFit="true"/>
+    <col min="76" max="76" width="33.77734375" customWidth="true" bestFit="true"/>
+    <col min="77" max="77" width="44.51171875" customWidth="true" bestFit="true"/>
+    <col min="78" max="78" width="41.6640625" customWidth="true" bestFit="true"/>
+    <col min="79" max="79" width="48.109375" customWidth="true" bestFit="true"/>
+    <col min="80" max="80" width="29.85546875" customWidth="true" bestFit="true"/>
+    <col min="81" max="81" width="22.90234375" customWidth="true" bestFit="true"/>
+    <col min="82" max="82" width="24.953125" customWidth="true" bestFit="true"/>
+    <col min="83" max="83" width="18.94921875" customWidth="true" bestFit="true"/>
+    <col min="84" max="84" width="20.7734375" customWidth="true" bestFit="true"/>
+    <col min="85" max="85" width="14.33984375" customWidth="true" bestFit="true"/>
+    <col min="86" max="86" width="2.07421875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>